<commit_message>
alteração na formatação da planilha de novembro
</commit_message>
<xml_diff>
--- a/WebContent/WEB-INF/classes/entrada-11-2020.xlsx
+++ b/WebContent/WEB-INF/classes/entrada-11-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luizorta/Dev/github/TimesheetClockifyFacilitator/WebContent/WEB-INF/classes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10F4B8D-8D21-244A-900D-9F4F7B446BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A8351D-3D81-2149-9DD8-BFFC0D5B3560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="90B7" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="30500" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -616,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -789,6 +789,15 @@
     <xf numFmtId="165" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,6 +813,39 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="46" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -837,47 +879,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1397,7 +1403,7 @@
   <dimension ref="B1:AG46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1431,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B1" s="68"/>
+      <c r="B1" s="71"/>
       <c r="C1" s="24"/>
       <c r="AA1" s="38" t="s">
         <v>19</v>
@@ -1449,7 +1455,7 @@
       </c>
     </row>
     <row r="2" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B2" s="69"/>
+      <c r="B2" s="72"/>
       <c r="C2" s="32"/>
       <c r="T2" s="36" t="s">
         <v>19</v>
@@ -1666,16 +1672,16 @@
       </c>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="95" t="s">
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="96"/>
-      <c r="G8" s="97"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="70"/>
       <c r="T8" s="37" t="s">
         <v>25</v>
       </c>
@@ -1862,7 +1868,7 @@
       </c>
     </row>
     <row r="13" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43">
+      <c r="B13" s="98">
         <v>0</v>
       </c>
       <c r="C13" s="44">
@@ -1873,7 +1879,7 @@
         <v>60</v>
       </c>
       <c r="E13" s="46"/>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G13" s="47"/>
@@ -1903,7 +1909,7 @@
       </c>
     </row>
     <row r="14" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="43">
+      <c r="B14" s="98">
         <v>0</v>
       </c>
       <c r="C14" s="44">
@@ -1914,7 +1920,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="46"/>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G14" s="47"/>
@@ -1938,7 +1944,7 @@
       </c>
     </row>
     <row r="15" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="43">
+      <c r="B15" s="98">
         <v>0</v>
       </c>
       <c r="C15" s="44">
@@ -1949,7 +1955,7 @@
         <v>60</v>
       </c>
       <c r="E15" s="46"/>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G15" s="47"/>
@@ -1973,14 +1979,14 @@
       </c>
     </row>
     <row r="16" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="53"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="54">
         <f t="shared" ca="1" si="2"/>
         <v>44142</v>
       </c>
       <c r="D16" s="55"/>
       <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="57" t="s">
         <v>57</v>
       </c>
@@ -2004,7 +2010,7 @@
       </c>
     </row>
     <row r="17" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="43">
+      <c r="B17" s="98">
         <v>0</v>
       </c>
       <c r="C17" s="44">
@@ -2015,7 +2021,7 @@
         <v>60</v>
       </c>
       <c r="E17" s="46"/>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G17" s="47"/>
@@ -2039,7 +2045,7 @@
       </c>
     </row>
     <row r="18" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43">
+      <c r="B18" s="98">
         <v>0</v>
       </c>
       <c r="C18" s="44">
@@ -2050,7 +2056,7 @@
         <v>60</v>
       </c>
       <c r="E18" s="46"/>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G18" s="47"/>
@@ -2074,7 +2080,7 @@
       </c>
     </row>
     <row r="19" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="43">
+      <c r="B19" s="98">
         <v>0</v>
       </c>
       <c r="C19" s="44">
@@ -2085,7 +2091,7 @@
         <v>60</v>
       </c>
       <c r="E19" s="46"/>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G19" s="47"/>
@@ -2109,7 +2115,7 @@
       </c>
     </row>
     <row r="20" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43">
+      <c r="B20" s="98">
         <v>0</v>
       </c>
       <c r="C20" s="44">
@@ -2120,7 +2126,7 @@
         <v>60</v>
       </c>
       <c r="E20" s="46"/>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G20" s="47"/>
@@ -2144,7 +2150,7 @@
       </c>
     </row>
     <row r="21" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="43">
+      <c r="B21" s="98">
         <v>0</v>
       </c>
       <c r="C21" s="44">
@@ -2155,7 +2161,7 @@
         <v>60</v>
       </c>
       <c r="E21" s="46"/>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G21" s="47"/>
@@ -2179,14 +2185,14 @@
       </c>
     </row>
     <row r="22" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="53"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="54">
         <f t="shared" ca="1" si="2"/>
         <v>44149</v>
       </c>
       <c r="D22" s="55"/>
       <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
+      <c r="F22" s="57"/>
       <c r="G22" s="57" t="s">
         <v>57</v>
       </c>
@@ -2210,7 +2216,7 @@
       </c>
     </row>
     <row r="23" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="43">
+      <c r="B23" s="98">
         <v>0</v>
       </c>
       <c r="C23" s="44">
@@ -2221,7 +2227,7 @@
         <v>60</v>
       </c>
       <c r="E23" s="46"/>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G23" s="47"/>
@@ -2245,7 +2251,7 @@
       </c>
     </row>
     <row r="24" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="43">
+      <c r="B24" s="98">
         <v>0</v>
       </c>
       <c r="C24" s="44">
@@ -2256,7 +2262,7 @@
         <v>60</v>
       </c>
       <c r="E24" s="46"/>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G24" s="47"/>
@@ -2280,7 +2286,7 @@
       </c>
     </row>
     <row r="25" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="43">
+      <c r="B25" s="98">
         <v>0</v>
       </c>
       <c r="C25" s="44">
@@ -2291,7 +2297,7 @@
         <v>60</v>
       </c>
       <c r="E25" s="46"/>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G25" s="47"/>
@@ -2315,7 +2321,7 @@
       </c>
     </row>
     <row r="26" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="43">
+      <c r="B26" s="98">
         <v>0</v>
       </c>
       <c r="C26" s="44">
@@ -2326,7 +2332,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="46"/>
-      <c r="F26" s="46" t="s">
+      <c r="F26" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G26" s="47"/>
@@ -2350,7 +2356,7 @@
       </c>
     </row>
     <row r="27" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43">
+      <c r="B27" s="98">
         <v>0</v>
       </c>
       <c r="C27" s="44">
@@ -2361,7 +2367,7 @@
         <v>60</v>
       </c>
       <c r="E27" s="46"/>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="47"/>
@@ -2385,14 +2391,14 @@
       </c>
     </row>
     <row r="28" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53"/>
+      <c r="B28" s="99"/>
       <c r="C28" s="54">
         <f t="shared" ca="1" si="2"/>
         <v>44156</v>
       </c>
       <c r="D28" s="55"/>
       <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
+      <c r="F28" s="57"/>
       <c r="G28" s="57" t="s">
         <v>57</v>
       </c>
@@ -2416,7 +2422,7 @@
       </c>
     </row>
     <row r="29" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43">
+      <c r="B29" s="98">
         <v>0</v>
       </c>
       <c r="C29" s="44">
@@ -2427,7 +2433,7 @@
         <v>60</v>
       </c>
       <c r="E29" s="46"/>
-      <c r="F29" s="46" t="s">
+      <c r="F29" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G29" s="47"/>
@@ -2794,35 +2800,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="86"/>
+      <c r="B1" s="78"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
+      <c r="B2" s="78"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
     </row>
     <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="77"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="F5" s="42" t="s">
         <v>1</v>
       </c>
@@ -2840,35 +2846,35 @@
     </row>
     <row r="6" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="87" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="93"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="M8" s="17"/>
@@ -2891,52 +2897,52 @@
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="91"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="90" t="s">
+      <c r="E12" s="83"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="91"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="90" t="s">
+      <c r="H12" s="83"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="91"/>
-      <c r="L12" s="92"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="84"/>
       <c r="M12" s="25"/>
-      <c r="N12" s="93" t="s">
+      <c r="N12" s="85" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
-      <c r="C13" s="83"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="25" t="s">
         <v>8</v>
       </c>
@@ -2967,7 +2973,7 @@
       <c r="M13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="N13" s="94"/>
+      <c r="N13" s="86"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="30">
@@ -3960,24 +3966,24 @@
       <c r="N44" s="20"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="74" t="s">
+      <c r="B45" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="75"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
       <c r="F45" s="26">
         <f>SUM(F14:F44)</f>
         <v>0</v>
       </c>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
       <c r="I45" s="26">
         <f>SUM(I14:I44)</f>
         <v>0</v>
       </c>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
       <c r="L45" s="26">
         <f>SUM(L14:L44)</f>
         <v>0</v>
@@ -4025,14 +4031,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D7:N7"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="N12:N13"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="J45:K45"/>
@@ -4042,6 +4040,14 @@
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D7:N7"/>
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="N12:N13"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C14:C44">

</xml_diff>